<commit_message>
Second commit - committing all files to the Repo
</commit_message>
<xml_diff>
--- a/graphics/mango2.xlsx
+++ b/graphics/mango2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACER\OneDrive - University of Moratuwa\My Docs\Research Papers\Conferences\2023-mango\graphics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyDocs\ResearchPapers\Journals\2024_mango\graphics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64D1005-D3AF-4C28-8810-ECEC1A750BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F2B21-8939-46B7-BDE5-AD3C63725AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A96F99A-6952-46F7-B2D1-B1401CA3C0D7}"/>
   </bookViews>
@@ -1408,7 +1408,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Day_28 (Spray_01)</c:v>
+            <c:v>Day_20 (Spray_01)</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -3331,8 +3331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84CB43FE-FF10-4C50-8397-DA859F95FCFE}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="V43" sqref="V43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -3653,12 +3653,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5690e09a-3277-447f-9d9d-5f4f29e47c6d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3915,17 +3914,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5690e09a-3277-447f-9d9d-5f4f29e47c6d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D765E32-E60F-42A2-8523-7CA1E0DB2E4A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7823C2E5-BDEB-4CB4-B913-522A95AC65AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="5690e09a-3277-447f-9d9d-5f4f29e47c6d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3428f634-e756-4d57-b4c3-2213e36291e5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3950,18 +3959,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7823C2E5-BDEB-4CB4-B913-522A95AC65AC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D765E32-E60F-42A2-8523-7CA1E0DB2E4A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5690e09a-3277-447f-9d9d-5f4f29e47c6d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3428f634-e756-4d57-b4c3-2213e36291e5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>